<commit_message>
Updated filtered search price ranges
Also corrected filtered search bugs
</commit_message>
<xml_diff>
--- a/Build Files/filteredsearch/Filtered Search exact values.xlsx
+++ b/Build Files/filteredsearch/Filtered Search exact values.xlsx
@@ -30,31 +30,16 @@
     <t>Wood Chess Sets with Boards</t>
   </si>
   <si>
-    <t>prod_type</t>
-  </si>
-  <si>
     <t>chesssets</t>
   </si>
   <si>
-    <t>prod_material</t>
-  </si>
-  <si>
     <t>woodwithboard</t>
   </si>
   <si>
-    <t>prod_king_height</t>
-  </si>
-  <si>
     <t>2.75, 3, 3.25, 3.5, 3.75, 3.875, 4, 4.125, 4.25, 4.4, 4.5, 4.75, 5</t>
   </si>
   <si>
-    <t>prod_wood_type</t>
-  </si>
-  <si>
     <t>black, boxwood, ebonizedboxwood, ebony, goldenrosewood, africanpadauk, red, redsandalwood, rosewood, white</t>
-  </si>
-  <si>
-    <t>prod_material_attribute_2</t>
   </si>
   <si>
     <r>
@@ -83,9 +68,6 @@
     </r>
   </si>
   <si>
-    <t>prod_model_type</t>
-  </si>
-  <si>
     <t>bridledstallion, british, columbianknight, deluxeoldclub, fierceknight, frenchlardy, germanknight, grande, kingsguard, khansstallion, newexclusive, parker, players, royal, stjohn, wellington, wingfield, yugoslavia</t>
   </si>
   <si>
@@ -101,9 +83,6 @@
     <t>boxwood, ebonizedboxwood, ebony, goldenrosewood, rosewood</t>
   </si>
   <si>
-    <t>prod_design_type</t>
-  </si>
-  <si>
     <t>drawers, lifttop, folding</t>
   </si>
   <si>
@@ -146,9 +125,6 @@
     <t>theme</t>
   </si>
   <si>
-    <t>prod_manufacturer</t>
-  </si>
-  <si>
     <t>crushedstone, metal, plastic, polystone</t>
   </si>
   <si>
@@ -305,15 +281,6 @@
     <t>Chess DVDs</t>
   </si>
   <si>
-    <t>prod_subject</t>
-  </si>
-  <si>
-    <t>prod_strategy</t>
-  </si>
-  <si>
-    <t>prod_publisher</t>
-  </si>
-  <si>
     <t>dvd</t>
   </si>
   <si>
@@ -336,6 +303,39 @@
   </si>
   <si>
     <t>gambit, everymanchess, firesidelibrary</t>
+  </si>
+  <si>
+    <t>user:prod_type</t>
+  </si>
+  <si>
+    <t>user:prod_material</t>
+  </si>
+  <si>
+    <t>user:prod_size</t>
+  </si>
+  <si>
+    <t>user:prod_mat_attrib_1</t>
+  </si>
+  <si>
+    <t>user:prod_model_type</t>
+  </si>
+  <si>
+    <t>user:prod_material_attrib_2</t>
+  </si>
+  <si>
+    <t>user:prod_manufacturer</t>
+  </si>
+  <si>
+    <t>user:prod_design_type</t>
+  </si>
+  <si>
+    <t>user:prod_subject</t>
+  </si>
+  <si>
+    <t>user:prod_strategy</t>
+  </si>
+  <si>
+    <t>user:prod_publisher</t>
   </si>
 </sst>
 </file>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -721,955 +721,955 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="B17" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="B18" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="B19" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
         <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="B24" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="B25" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="B26" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
         <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="B32" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
         <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="B35" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="B37" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="B41" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="B49" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C51" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="B52" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="B53" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="B54" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C56" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="B57" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="B58" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="B59" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C62" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="B63" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="B64" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="B66" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C68" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="B69" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="B70" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="B71" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="B72" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C74" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="B75" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="B76" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="B77" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="B78" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C80" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="B81" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="B82" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="B83" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="B84" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="B87" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="B88" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="B89" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="B92" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="B93" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="B94" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="B95" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C97" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="B98" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C98" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="B99" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="B100" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C102" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="B103" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C103" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="B104" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="B105" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="B106" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C108" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="B109" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C109" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="B110" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="B111" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="B112" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C114" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="B115" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C115" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="B116" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="B117" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="B118" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C120" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="B121" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C121" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="B122" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="B123" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B125" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C125" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="B126" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C126" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="B127" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="45" customHeight="1">
       <c r="B128" s="3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="B129" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C131" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="B132" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C132" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="B133" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="45">
       <c r="B134" s="3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="B135" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>